<commit_message>
Updated 3 types of files
</commit_message>
<xml_diff>
--- a/Login test case.xlsx
+++ b/Login test case.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>slno</t>
   </si>
@@ -60,6 +60,21 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>login with valid cred</t>
+  </si>
+  <si>
+    <t>user should be in login scree</t>
+  </si>
+  <si>
+    <t>Enter valid UserName and Password then click on login button</t>
+  </si>
+  <si>
+    <t>User should be able to enter user name and password</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -72,14 +87,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,148 +543,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1001,15 +1009,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
-    <col min="2" max="2" width="12.8888888888889" customWidth="1"/>
+    <col min="2" max="2" width="17.7777777777778" customWidth="1"/>
     <col min="3" max="3" width="29.4444444444444" customWidth="1"/>
     <col min="4" max="4" width="26.4444444444444" customWidth="1"/>
     <col min="5" max="5" width="47.2222222222222" customWidth="1"/>
@@ -1056,6 +1064,26 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>